<commit_message>
update check in to allow many rooms
</commit_message>
<xml_diff>
--- a/booking.xlsx
+++ b/booking.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25831"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USER\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="d:\Users\apnev\Documents\GitHub\hotel_database\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{684F112D-AB28-489A-A52F-085B40B9A9EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{122946D0-9018-4427-B983-B87014C7E065}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8004" yWindow="504" windowWidth="13704" windowHeight="10860" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="32535" yWindow="1815" windowWidth="21690" windowHeight="11235" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="14">
   <si>
     <t>booking_id</t>
   </si>
@@ -111,14 +111,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Κανονικό" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -396,10 +394,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K14"/>
+  <dimension ref="A1:K15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="N13" sqref="N13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M15" sqref="M15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -461,7 +459,7 @@
       <c r="D2" s="1">
         <v>44658</v>
       </c>
-      <c r="E2" s="2">
+      <c r="E2">
         <f xml:space="preserve"> (20*B2)/100</f>
         <v>24</v>
       </c>
@@ -480,7 +478,7 @@
       <c r="J2">
         <v>1</v>
       </c>
-      <c r="K2" s="3">
+      <c r="K2">
         <v>153428961</v>
       </c>
     </row>
@@ -533,8 +531,8 @@
       <c r="D4" s="1">
         <v>44871</v>
       </c>
-      <c r="E4" s="2">
-        <f t="shared" ref="E4:E14" si="0" xml:space="preserve"> (20*B4)/100</f>
+      <c r="E4">
+        <f t="shared" ref="E4:E15" si="0" xml:space="preserve"> (20*B4)/100</f>
         <v>60</v>
       </c>
       <c r="F4">
@@ -569,7 +567,7 @@
       <c r="D5" s="1">
         <v>44858</v>
       </c>
-      <c r="E5" s="2">
+      <c r="E5">
         <f t="shared" si="0"/>
         <v>48</v>
       </c>
@@ -605,7 +603,7 @@
       <c r="D6" s="1">
         <v>44767</v>
       </c>
-      <c r="E6" s="2">
+      <c r="E6">
         <f t="shared" si="0"/>
         <v>120</v>
       </c>
@@ -641,7 +639,7 @@
       <c r="D7" s="1">
         <v>44781</v>
       </c>
-      <c r="E7" s="2">
+      <c r="E7">
         <f t="shared" si="0"/>
         <v>156</v>
       </c>
@@ -660,7 +658,7 @@
       <c r="J7">
         <v>2</v>
       </c>
-      <c r="K7" s="2">
+      <c r="K7">
         <v>151546513</v>
       </c>
     </row>
@@ -696,7 +694,7 @@
       <c r="J8">
         <v>1</v>
       </c>
-      <c r="K8" s="2">
+      <c r="K8">
         <v>107290304</v>
       </c>
     </row>
@@ -914,6 +912,42 @@
       </c>
       <c r="K14">
         <v>106123465</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15">
+        <v>320</v>
+      </c>
+      <c r="C15" s="1">
+        <v>44930</v>
+      </c>
+      <c r="D15" s="1">
+        <v>44932</v>
+      </c>
+      <c r="E15">
+        <f t="shared" si="0"/>
+        <v>64</v>
+      </c>
+      <c r="F15">
+        <v>64</v>
+      </c>
+      <c r="G15" s="1">
+        <v>44916</v>
+      </c>
+      <c r="H15" t="s">
+        <v>11</v>
+      </c>
+      <c r="I15">
+        <v>0</v>
+      </c>
+      <c r="J15">
+        <v>4</v>
+      </c>
+      <c r="K15">
+        <v>107275663</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Show late downpayments (individuals)
</commit_message>
<xml_diff>
--- a/booking.xlsx
+++ b/booking.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="d:\Users\apnev\Documents\GitHub\hotel_database\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{122946D0-9018-4427-B983-B87014C7E065}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{188358ED-720B-4433-B7BD-02FCBB6C6997}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="32535" yWindow="1815" windowWidth="21690" windowHeight="11235" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="40755" yWindow="1710" windowWidth="21690" windowHeight="11235" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -397,7 +397,7 @@
   <dimension ref="A1:K15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M15" sqref="M15"/>
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -932,7 +932,7 @@
         <v>64</v>
       </c>
       <c r="F15">
-        <v>64</v>
+        <v>0</v>
       </c>
       <c r="G15" s="1">
         <v>44916</v>

</xml_diff>

<commit_message>
Show late downpayments (agencies)
</commit_message>
<xml_diff>
--- a/booking.xlsx
+++ b/booking.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="d:\Users\apnev\Documents\GitHub\hotel_database\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{188358ED-720B-4433-B7BD-02FCBB6C6997}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A786E792-9E1E-4EA0-A6E5-199BCD6DCE3E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="40755" yWindow="1710" windowWidth="21690" windowHeight="11235" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="14">
   <si>
     <t>booking_id</t>
   </si>
@@ -394,10 +394,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K15"/>
+  <dimension ref="A1:K16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -532,7 +532,7 @@
         <v>44871</v>
       </c>
       <c r="E4">
-        <f t="shared" ref="E4:E15" si="0" xml:space="preserve"> (20*B4)/100</f>
+        <f t="shared" ref="E4:E16" si="0" xml:space="preserve"> (20*B4)/100</f>
         <v>60</v>
       </c>
       <c r="F4">
@@ -948,6 +948,42 @@
       </c>
       <c r="K15">
         <v>107275663</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16">
+        <v>320</v>
+      </c>
+      <c r="C16" s="1">
+        <v>44930</v>
+      </c>
+      <c r="D16" s="1">
+        <v>44932</v>
+      </c>
+      <c r="E16">
+        <f t="shared" si="0"/>
+        <v>64</v>
+      </c>
+      <c r="F16">
+        <v>0</v>
+      </c>
+      <c r="G16" s="1">
+        <v>44916</v>
+      </c>
+      <c r="H16" t="s">
+        <v>12</v>
+      </c>
+      <c r="I16">
+        <v>2</v>
+      </c>
+      <c r="J16">
+        <v>2</v>
+      </c>
+      <c r="K16">
+        <v>569784126</v>
       </c>
     </row>
   </sheetData>

</xml_diff>